<commit_message>
25.04.2018 - szkoła update
</commit_message>
<xml_diff>
--- a/informatyka/Filip Perz Wykresy/Wykresy-4.xlsx
+++ b/informatyka/Filip Perz Wykresy/Wykresy-4.xlsx
@@ -1,16 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEM\Documents\GitHub\wszystkoSzkola\informatyka\Filip Perz Wykresy\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6060BAE4-D459-46DA-A904-C0089F67069F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="11340" windowHeight="6540"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="11340" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wykres1" sheetId="2" r:id="rId1"/>
     <sheet name="Wykres2" sheetId="5" r:id="rId2"/>
+    <sheet name="Wykres3" sheetId="7" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -56,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -364,8 +371,2429 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Przebieg</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Wykres1!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kwadraty</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Wykres1!$C$8:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002A-795D-4E4C-A054-6A645D325D1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Wykres1!$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sumy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Wykres1!$D$8:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>260</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002B-795D-4E4C-A054-6A645D325D1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1530235567"/>
+        <c:axId val="1531754927"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Wykres1!$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Liczby naturalne</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Wykres1!$A$8:$A$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>14</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000028-795D-4E4C-A054-6A645D325D1C}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1530235567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Liczby</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> naturalne</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.42643893078319894"/>
+              <c:y val="0.88331000291630213"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1531754927"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1531754927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Wartości</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1530235567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.7699115044247787E-2"/>
+          <c:y val="0.59598279381743946"/>
+          <c:w val="0.20519266950038326"/>
+          <c:h val="0.32696923301254011"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Wzrost</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.39368744531933514"/>
+          <c:y val="4.3290043290043288E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.5274692014849496E-2"/>
+          <c:y val="0.1399973606651124"/>
+          <c:w val="0.78509805497261043"/>
+          <c:h val="0.6399853427412483"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Seria 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:shade val="51000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="80000">
+                  <a:schemeClr val="accent3">
+                    <a:shade val="93000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:shade val="94000"/>
+                    <a:satMod val="135000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Wykres2!$C$6:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C38F-47C8-B00F-3EC1A7810AEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Seria 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="51000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="80000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="93000"/>
+                    <a:satMod val="130000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="94000"/>
+                    <a:satMod val="135000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Wykres2!$D$6:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>260</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C38F-47C8-B00F-3EC1A7810AEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="1528936575"/>
+        <c:axId val="1711386383"/>
+        <c:extLst/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1528936575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>W</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>artosci</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1711386383"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1711386383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Zasięg</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44987379702537178"/>
+              <c:y val="0.85148462587427964"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1528936575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="220">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{75C300F5-51AE-47A0-A559-82AE62E97FA8}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C353A98-8E0F-4D0E-BA38-C47DCBD2E88E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F593DD3-0621-4A39-9E96-B16A8650402F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,7 +2839,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -444,9 +2872,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -479,6 +2924,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -654,11 +3116,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -914,15 +3376,16 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>